<commit_message>
Solve the NA to as.numeric problem
</commit_message>
<xml_diff>
--- a/CuaaQualityRanking.xlsx
+++ b/CuaaQualityRanking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="922" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="922" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="2009" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9725" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9725" uniqueCount="857">
   <si>
     <t>学校名称</t>
   </si>
@@ -2458,9 +2458,6 @@
   </si>
   <si>
     <t>北京建筑大学</t>
-  </si>
-  <si>
-    <t>地区</t>
   </si>
   <si>
     <t>社会影响</t>
@@ -47029,7 +47026,7 @@
   </sheetPr>
   <dimension ref="A1:G301"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A278" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -53980,8 +53977,8 @@
   </sheetPr>
   <dimension ref="A1:G301"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A145" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -53990,7 +53987,7 @@
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -53998,7 +53995,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>790</v>
+        <v>381</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -54010,7 +54007,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54222,7 +54219,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>11</v>
@@ -55234,7 +55231,7 @@
     </row>
     <row r="55" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>11</v>
@@ -55303,7 +55300,7 @@
     </row>
     <row r="58" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>127</v>
@@ -55372,7 +55369,7 @@
     </row>
     <row r="61" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>127</v>
@@ -55464,7 +55461,7 @@
     </row>
     <row r="65" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>127</v>
@@ -55970,7 +55967,7 @@
     </row>
     <row r="87" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="5" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>11</v>
@@ -60087,7 +60084,7 @@
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="8" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B266" s="8" t="s">
         <v>113</v>
@@ -60202,7 +60199,7 @@
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="8" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B271" s="8" t="s">
         <v>113</v>
@@ -60570,7 +60567,7 @@
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="8" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B287" s="8" t="s">
         <v>113</v>
@@ -60931,7 +60928,7 @@
   </sheetPr>
   <dimension ref="A1:G716"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -60965,7 +60962,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -61154,7 +61151,7 @@
     </row>
     <row r="10" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>11</v>
@@ -62212,7 +62209,7 @@
     </row>
     <row r="56" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="14" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>11</v>
@@ -62557,7 +62554,7 @@
     </row>
     <row r="71" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="14" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B71" s="14" t="s">
         <v>127</v>
@@ -62580,7 +62577,7 @@
     </row>
     <row r="72" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="14" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B72" s="14" t="s">
         <v>127</v>
@@ -62626,7 +62623,7 @@
     </row>
     <row r="74" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="14" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B74" s="14" t="s">
         <v>127</v>
@@ -62810,7 +62807,7 @@
     </row>
     <row r="82" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="14" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B82" s="14" t="s">
         <v>11</v>
@@ -67203,7 +67200,7 @@
     </row>
     <row r="273" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="14" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B273" s="14" t="s">
         <v>113</v>
@@ -67318,7 +67315,7 @@
     </row>
     <row r="278" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="14" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B278" s="14" t="s">
         <v>11</v>
@@ -67456,7 +67453,7 @@
     </row>
     <row r="284" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="14" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B284" s="14" t="s">
         <v>113</v>
@@ -67893,7 +67890,7 @@
     </row>
     <row r="303" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="14" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B303" s="14" t="s">
         <v>113</v>
@@ -68031,7 +68028,7 @@
     </row>
     <row r="309" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="14" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B309" s="14" t="s">
         <v>11</v>
@@ -68146,7 +68143,7 @@
     </row>
     <row r="314" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="14" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B314" s="14" t="s">
         <v>108</v>
@@ -68353,7 +68350,7 @@
     </row>
     <row r="323" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="14" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B323" s="14" t="s">
         <v>127</v>
@@ -68675,7 +68672,7 @@
     </row>
     <row r="337" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="14" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B337" s="14" t="s">
         <v>127</v>
@@ -68721,7 +68718,7 @@
     </row>
     <row r="339" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="14" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B339" s="14" t="s">
         <v>11</v>
@@ -68882,7 +68879,7 @@
     </row>
     <row r="346" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="14" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B346" s="14" t="s">
         <v>11</v>
@@ -68905,7 +68902,7 @@
     </row>
     <row r="347" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="14" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B347" s="14" t="s">
         <v>127</v>
@@ -69204,7 +69201,7 @@
     </row>
     <row r="360" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="14" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B360" s="14" t="s">
         <v>108</v>
@@ -69365,7 +69362,7 @@
     </row>
     <row r="367" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="14" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B367" s="14" t="s">
         <v>11</v>
@@ -69434,7 +69431,7 @@
     </row>
     <row r="370" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="14" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B370" s="14" t="s">
         <v>11</v>
@@ -70630,7 +70627,7 @@
     </row>
     <row r="422" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="14" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B422" s="14" t="s">
         <v>113</v>
@@ -70676,7 +70673,7 @@
     </row>
     <row r="424" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="14" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B424" s="14" t="s">
         <v>32</v>
@@ -70699,7 +70696,7 @@
     </row>
     <row r="425" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="14" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B425" s="14" t="s">
         <v>127</v>
@@ -70998,7 +70995,7 @@
     </row>
     <row r="438" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="14" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B438" s="14" t="s">
         <v>32</v>
@@ -71021,7 +71018,7 @@
     </row>
     <row r="439" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="14" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B439" s="14" t="s">
         <v>127</v>
@@ -71044,7 +71041,7 @@
     </row>
     <row r="440" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="14" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B440" s="14" t="s">
         <v>9</v>
@@ -71366,7 +71363,7 @@
     </row>
     <row r="454" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="14" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B454" s="14" t="s">
         <v>11</v>
@@ -71389,7 +71386,7 @@
     </row>
     <row r="455" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="14" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B455" s="14" t="s">
         <v>11</v>
@@ -71458,7 +71455,7 @@
     </row>
     <row r="458" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="14" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B458" s="14" t="s">
         <v>11</v>
@@ -71481,7 +71478,7 @@
     </row>
     <row r="459" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="14" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B459" s="14" t="s">
         <v>11</v>
@@ -72125,7 +72122,7 @@
     </row>
     <row r="487" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="14" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B487" s="14" t="s">
         <v>113</v>
@@ -72194,7 +72191,7 @@
     </row>
     <row r="490" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="14" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B490" s="14" t="s">
         <v>127</v>
@@ -72263,7 +72260,7 @@
     </row>
     <row r="493" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="14" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B493" s="14" t="s">
         <v>32</v>
@@ -72516,7 +72513,7 @@
     </row>
     <row r="504" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="14" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B504" s="14" t="s">
         <v>11</v>
@@ -73965,7 +73962,7 @@
     </row>
     <row r="567" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A567" s="14" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B567" s="14" t="s">
         <v>11</v>
@@ -74126,7 +74123,7 @@
     </row>
     <row r="574" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A574" s="14" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B574" s="14" t="s">
         <v>11</v>
@@ -74931,7 +74928,7 @@
     </row>
     <row r="609" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A609" s="14" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B609" s="14" t="s">
         <v>9</v>
@@ -75023,7 +75020,7 @@
     </row>
     <row r="613" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A613" s="14" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B613" s="14" t="s">
         <v>50</v>
@@ -75184,7 +75181,7 @@
     </row>
     <row r="620" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A620" s="14" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B620" s="14" t="s">
         <v>9</v>
@@ -75552,7 +75549,7 @@
     </row>
     <row r="636" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A636" s="14" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B636" s="14" t="s">
         <v>9</v>
@@ -75782,7 +75779,7 @@
     </row>
     <row r="646" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="14" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B646" s="14" t="s">
         <v>11</v>
@@ -75805,7 +75802,7 @@
     </row>
     <row r="647" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="14" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B647" s="14" t="s">
         <v>32</v>
@@ -75943,7 +75940,7 @@
     </row>
     <row r="653" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A653" s="14" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B653" s="14" t="s">
         <v>11</v>
@@ -76012,7 +76009,7 @@
     </row>
     <row r="656" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="14" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B656" s="14" t="s">
         <v>32</v>
@@ -76104,7 +76101,7 @@
     </row>
     <row r="660" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A660" s="14" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B660" s="14" t="s">
         <v>113</v>
@@ -76196,7 +76193,7 @@
     </row>
     <row r="664" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="14" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B664" s="14" t="s">
         <v>127</v>
@@ -76380,7 +76377,7 @@
     </row>
     <row r="672" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="14" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B672" s="14" t="s">
         <v>32</v>
@@ -76449,7 +76446,7 @@
     </row>
     <row r="675" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A675" s="14" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B675" s="14" t="s">
         <v>113</v>
@@ -76472,7 +76469,7 @@
     </row>
     <row r="676" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A676" s="14" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B676" s="14" t="s">
         <v>32</v>
@@ -76633,7 +76630,7 @@
     </row>
     <row r="683" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="14" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B683" s="14" t="s">
         <v>32</v>
@@ -76702,7 +76699,7 @@
     </row>
     <row r="686" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A686" s="14" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B686" s="14" t="s">
         <v>9</v>
@@ -76794,7 +76791,7 @@
     </row>
     <row r="690" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A690" s="14" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B690" s="14" t="s">
         <v>9</v>
@@ -76817,7 +76814,7 @@
     </row>
     <row r="691" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A691" s="14" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B691" s="14" t="s">
         <v>9</v>
@@ -77024,7 +77021,7 @@
     </row>
     <row r="700" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A700" s="14" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B700" s="14" t="s">
         <v>50</v>
@@ -77093,7 +77090,7 @@
     </row>
     <row r="703" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A703" s="14" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B703" s="14" t="s">
         <v>32</v>
@@ -77116,7 +77113,7 @@
     </row>
     <row r="704" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A704" s="14" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B704" s="14" t="s">
         <v>127</v>
@@ -77139,7 +77136,7 @@
     </row>
     <row r="705" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A705" s="14" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B705" s="14" t="s">
         <v>113</v>
@@ -77162,7 +77159,7 @@
     </row>
     <row r="706" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A706" s="14" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B706" s="14" t="s">
         <v>32</v>
@@ -77185,7 +77182,7 @@
     </row>
     <row r="707" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A707" s="14" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B707" s="14" t="s">
         <v>11</v>
@@ -77208,7 +77205,7 @@
     </row>
     <row r="708" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A708" s="14" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B708" s="14" t="s">
         <v>32</v>
@@ -77231,7 +77228,7 @@
     </row>
     <row r="709" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A709" s="14" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B709" s="14" t="s">
         <v>127</v>
@@ -77254,7 +77251,7 @@
     </row>
     <row r="710" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A710" s="14" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B710" s="14" t="s">
         <v>127</v>
@@ -77300,7 +77297,7 @@
     </row>
     <row r="712" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A712" s="14" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B712" s="14" t="s">
         <v>113</v>
@@ -77323,7 +77320,7 @@
     </row>
     <row r="713" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A713" s="14" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B713" s="14" t="s">
         <v>11</v>
@@ -77346,7 +77343,7 @@
     </row>
     <row r="714" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A714" s="14" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B714" s="14" t="s">
         <v>11</v>
@@ -77369,7 +77366,7 @@
     </row>
     <row r="715" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A715" s="14" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B715" s="14" t="s">
         <v>32</v>

</xml_diff>